<commit_message>
Lấy xong dữ liệu data và dữ liệu lỗi
</commit_message>
<xml_diff>
--- a/QA_REPORT_MONTHLY/GUI/bin/Debug/CONFIG/config_qa_report_monthly.xlsx
+++ b/QA_REPORT_MONTHLY/GUI/bin/Debug/CONFIG/config_qa_report_monthly.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sys009\Desktop\Hoai_Daotao\vs\QA\PROJECT\QA_REPORT_MONTHLY\GUI\bin\Debug\CONFIG\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8141F993-91A6-435C-9E2D-DDB0278401D3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1ADF2868-E3B6-4362-A0C0-EE6BB4DF6F74}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Key</t>
   </si>
@@ -48,16 +48,22 @@
     <t>SourceFileError</t>
   </si>
   <si>
-    <t>P:\96. Share Data\99. Other\13. IT\HOAI\QA_REPORT\NGUON\1.Bieu thong ke loi hang ngay 1.2023.xlsm</t>
-  </si>
-  <si>
     <t>P:\96. Share Data\99. Other\13. IT\HOAI\QA_REPORT\NGUON\3.IN FORM G2 + DỮ LIỆU G2( NEW).xlsx</t>
   </si>
   <si>
     <t>FileError_SheetName</t>
   </si>
   <si>
-    <t>Total</t>
+    <t>FileError_Password</t>
+  </si>
+  <si>
+    <t>2357</t>
+  </si>
+  <si>
+    <t>P:\96. Share Data\99. Other\13. IT\HOAI\QA_REPORT\NGUON\2.Bieu thong ke loi hang ngay 2.2023(New).xlsm</t>
+  </si>
+  <si>
+    <t>Main</t>
   </si>
 </sst>
 </file>
@@ -93,8 +99,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -375,10 +382,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -400,7 +407,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -408,14 +415,22 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>6</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B5" s="1" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Check voi chi Dung tương doi on
</commit_message>
<xml_diff>
--- a/QA_REPORT_MONTHLY/GUI/bin/Debug/CONFIG/config_qa_report_monthly.xlsx
+++ b/QA_REPORT_MONTHLY/GUI/bin/Debug/CONFIG/config_qa_report_monthly.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sys009\Desktop\Hoai_Daotao\vs\QA\PROJECT\QA_REPORT_MONTHLY\GUI\bin\Debug\CONFIG\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\hoai\Hoai_Daotao\vs\QA\PROJECT\QA_REPORT_MONTHLY\GUI\bin\Debug\CONFIG\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8006B27C-5735-4A11-92FE-AFB3DA49FABB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A37ED91-4C7E-4493-A954-5CBF84506206}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5865" yWindow="1590" windowWidth="19200" windowHeight="14760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -48,9 +48,6 @@
     <t>SourceFileError</t>
   </si>
   <si>
-    <t>P:\96. Share Data\99. Other\13. IT\HOAI\QA_REPORT\NGUON\3.IN FORM G2 + DỮ LIỆU G2( NEW).xlsx</t>
-  </si>
-  <si>
     <t>FileError_SheetName</t>
   </si>
   <si>
@@ -60,9 +57,6 @@
     <t>2357</t>
   </si>
   <si>
-    <t>P:\96. Share Data\99. Other\13. IT\HOAI\QA_REPORT\NGUON\2.Bieu thong ke loi hang ngay 2.2023(New).xlsm</t>
-  </si>
-  <si>
     <t>Main</t>
   </si>
   <si>
@@ -70,16 +64,30 @@
   </si>
   <si>
     <t>\CONFIG\Template.xlsx</t>
+  </si>
+  <si>
+    <t>P:\96. Share Data\99. Other\13. IT\HOAI\QA_REPORT\HOAISFSF\3.IN FORM G2 + DỮ LIỆU G2( NEW).xlsx</t>
+  </si>
+  <si>
+    <t>P:\96. Share Data\99. Other\60 QA\006.NHAP_LOI_HANG_NGAY(QA)\02.Nam_2023\2.Bieu thong ke loi hang ngay 2.2023(New).xlsm</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -102,14 +110,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -391,7 +402,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -412,8 +423,8 @@
       <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
-        <v>4</v>
+      <c r="B2" s="2" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -421,34 +432,37 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B6" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" display="\\192.168.3.6\public\60. Quality Control\29. G2\1. G2_NM1\3.IN FORM G2 + DỮ LIỆU G2( NEW).xlsx" xr:uid="{B7096B56-9FFD-4EA0-99CF-422FDBF088AF}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Tuong doi on phan 2
</commit_message>
<xml_diff>
--- a/QA_REPORT_MONTHLY/GUI/bin/Debug/CONFIG/config_qa_report_monthly.xlsx
+++ b/QA_REPORT_MONTHLY/GUI/bin/Debug/CONFIG/config_qa_report_monthly.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\hoai\Hoai_Daotao\vs\QA\PROJECT\QA_REPORT_MONTHLY\GUI\bin\Debug\CONFIG\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46BA023A-7A0E-4237-A7CC-358369093F14}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48F90226-66C2-47A4-B1E5-F50A4D6FEB4A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Key</t>
   </si>
@@ -76,6 +76,12 @@
   </si>
   <si>
     <t>B</t>
+  </si>
+  <si>
+    <t>2FileTemplate</t>
+  </si>
+  <si>
+    <t>\CONFIG\Template_kyocera_2.xlsx</t>
   </si>
 </sst>
 </file>
@@ -405,10 +411,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -473,6 +479,14 @@
         <v>13</v>
       </c>
     </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" t="s">
+        <v>15</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" display="\\192.168.3.6\public\60. Quality Control\29. G2\1. G2_NM1\3.IN FORM G2 + DỮ LIỆU G2( NEW).xlsx" xr:uid="{B7096B56-9FFD-4EA0-99CF-422FDBF088AF}"/>

</xml_diff>

<commit_message>
Đang làm QA Report Monthly
</commit_message>
<xml_diff>
--- a/QA_REPORT_MONTHLY/GUI/bin/Debug/CONFIG/config_qa_report_monthly.xlsx
+++ b/QA_REPORT_MONTHLY/GUI/bin/Debug/CONFIG/config_qa_report_monthly.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\hoai\Hoai_Daotao\vs\QA\PROJECT\QA_REPORT_MONTHLY\GUI\bin\Debug\CONFIG\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48F90226-66C2-47A4-B1E5-F50A4D6FEB4A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DC85EC2-4683-4415-A921-9FE2DAF164EB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
   <si>
     <t>Key</t>
   </si>
@@ -82,6 +82,9 @@
   </si>
   <si>
     <t>\CONFIG\Template_kyocera_2.xlsx</t>
+  </si>
+  <si>
+    <t>3ColumnModel</t>
   </si>
 </sst>
 </file>
@@ -411,10 +414,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -487,6 +490,14 @@
         <v>15</v>
       </c>
     </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" t="s">
+        <v>13</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" display="\\192.168.3.6\public\60. Quality Control\29. G2\1. G2_NM1\3.IN FORM G2 + DỮ LIỆU G2( NEW).xlsx" xr:uid="{B7096B56-9FFD-4EA0-99CF-422FDBF088AF}"/>

</xml_diff>